<commit_message>
Cleaned project, renamed files, created PCA
</commit_message>
<xml_diff>
--- a/2.Data/VegetationData.xlsx
+++ b/2.Data/VegetationData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/evert_sprockel_wur_nl/Documents/5.Wageningen/7.Thesis/7.DataAnalysis/RScripts/2.Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/evert_sprockel_wur_nl/Documents/5.Wageningen/7.Thesis/7.DataAnalysis/ThesisRAnalysis/2.Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="587" documentId="8_{872A76ED-DD01-460B-A727-DB46B93C166B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{934939DF-02FD-47BC-9A3C-F65F63100FF1}"/>
+  <xr:revisionPtr revIDLastSave="593" documentId="8_{872A76ED-DD01-460B-A727-DB46B93C166B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4076D442-7596-46FB-ADC0-39DDDDFCCFDE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DACF362B-6137-4498-953D-1E748F44EEF0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="126">
   <si>
     <t>Blysmus kompressus</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Triglochin palustris</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Cyperaceae</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
   </si>
   <si>
     <t>Poaceae unknown</t>
-  </si>
-  <si>
-    <t>Juncaginaceae unknown</t>
   </si>
   <si>
     <t>Cyperaceae unknown</t>
@@ -574,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -606,6 +600,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,13 +935,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6620C268-8E80-43C7-B6DC-8822E5B4B5D3}">
-  <dimension ref="A1:DD210"/>
+  <dimension ref="A1:DD208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BH2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BS19" sqref="BS19"/>
+      <selection pane="bottomRight" activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,290 +952,290 @@
     <col min="96" max="96" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:93" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AI1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BK1" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="BK1" s="9" t="s">
+      <c r="BM1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BU1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BW1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BX1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="BY1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="CA1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="CB1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="CC1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CD1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CF1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="CM1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="CN1" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:92" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -1340,13 +1335,14 @@
       <c r="CL2" s="6"/>
       <c r="CM2" s="6"/>
       <c r="CN2" s="6"/>
-    </row>
-    <row r="3" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="CO2" s="19"/>
+    </row>
+    <row r="3" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -1447,12 +1443,12 @@
       <c r="CM3" s="6"/>
       <c r="CN3" s="6"/>
     </row>
-    <row r="4" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1563,12 +1559,12 @@
       <c r="CM4" s="6"/>
       <c r="CN4" s="6"/>
     </row>
-    <row r="5" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1711,12 +1707,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6">
@@ -1865,12 +1861,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1979,12 +1975,12 @@
       <c r="CM7" s="6"/>
       <c r="CN7" s="6"/>
     </row>
-    <row r="8" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -2095,12 +2091,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -2199,12 +2195,12 @@
       <c r="CM9" s="6"/>
       <c r="CN9" s="6"/>
     </row>
-    <row r="10" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -2311,12 +2307,12 @@
       <c r="CM10" s="6"/>
       <c r="CN10" s="6"/>
     </row>
-    <row r="11" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -2411,12 +2407,12 @@
       <c r="CM11" s="6"/>
       <c r="CN11" s="6"/>
     </row>
-    <row r="12" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -2511,12 +2507,12 @@
       <c r="CM12" s="6"/>
       <c r="CN12" s="6"/>
     </row>
-    <row r="13" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -2613,12 +2609,12 @@
       <c r="CM13" s="6"/>
       <c r="CN13" s="6"/>
     </row>
-    <row r="14" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2731,12 +2727,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -2839,12 +2835,12 @@
       <c r="CM15" s="6"/>
       <c r="CN15" s="6"/>
     </row>
-    <row r="16" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="7">
         <v>90</v>
@@ -3020,7 +3016,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -3146,7 +3142,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -3284,7 +3280,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7">
@@ -3424,7 +3420,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -3563,10 +3559,10 @@
     </row>
     <row r="21" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -3682,7 +3678,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -3808,7 +3804,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="6">
         <v>5</v>
@@ -3962,126 +3958,136 @@
       <c r="CN23" s="6"/>
     </row>
     <row r="24" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>27</v>
+      <c r="A24" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="B24" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7">
+        <v>20</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7">
+        <v>40</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7">
+        <v>3</v>
+      </c>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
+      <c r="AE24" s="7">
+        <v>40</v>
+      </c>
+      <c r="AF24" s="7"/>
+      <c r="AG24" s="7"/>
+      <c r="AH24" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="AI24" s="7"/>
+      <c r="AJ24" s="7"/>
+      <c r="AK24" s="7"/>
+      <c r="AL24" s="7"/>
+      <c r="AM24" s="7"/>
+      <c r="AN24" s="7"/>
+      <c r="AO24" s="7"/>
+      <c r="AP24" s="7"/>
+      <c r="AQ24" s="7"/>
+      <c r="AR24" s="7"/>
+      <c r="AS24" s="7"/>
+      <c r="AT24" s="7">
+        <v>5</v>
+      </c>
+      <c r="AU24" s="7"/>
+      <c r="AV24" s="7"/>
+      <c r="AW24" s="7"/>
+      <c r="AX24" s="7"/>
+      <c r="AY24" s="7"/>
+      <c r="AZ24" s="7"/>
+      <c r="BA24" s="7"/>
+      <c r="BB24" s="7"/>
+      <c r="BC24" s="7"/>
+      <c r="BD24" s="7"/>
+      <c r="BE24" s="7"/>
+      <c r="BF24" s="7"/>
+      <c r="BG24" s="7"/>
+      <c r="BH24" s="7"/>
+      <c r="BI24" s="7"/>
+      <c r="BJ24" s="7"/>
+      <c r="BK24" s="7">
         <v>25</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6"/>
-      <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
-      <c r="W24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="6"/>
-      <c r="AC24" s="6"/>
-      <c r="AD24" s="6"/>
-      <c r="AE24" s="6"/>
-      <c r="AF24" s="6"/>
-      <c r="AG24" s="6"/>
-      <c r="AH24" s="6"/>
-      <c r="AI24" s="6"/>
-      <c r="AJ24" s="6"/>
-      <c r="AK24" s="6"/>
-      <c r="AL24" s="6"/>
-      <c r="AM24" s="6"/>
-      <c r="AN24" s="6"/>
-      <c r="AO24" s="6"/>
-      <c r="AP24" s="6"/>
-      <c r="AQ24" s="6"/>
-      <c r="AR24" s="6"/>
-      <c r="AS24" s="6"/>
-      <c r="AT24" s="6"/>
-      <c r="AU24" s="6"/>
-      <c r="AV24" s="6"/>
-      <c r="AW24" s="6"/>
-      <c r="AX24" s="6"/>
-      <c r="AY24" s="6"/>
-      <c r="AZ24" s="6"/>
-      <c r="BA24" s="6"/>
-      <c r="BB24" s="6"/>
-      <c r="BC24" s="6"/>
-      <c r="BD24" s="6"/>
-      <c r="BE24" s="6"/>
-      <c r="BF24" s="6"/>
-      <c r="BG24" s="6"/>
-      <c r="BH24" s="6"/>
-      <c r="BI24" s="6"/>
-      <c r="BJ24" s="6"/>
-      <c r="BK24" s="6"/>
-      <c r="BL24" s="6"/>
-      <c r="BM24" s="6"/>
-      <c r="BN24" s="6"/>
-      <c r="BO24" s="6"/>
-      <c r="BP24" s="6"/>
-      <c r="BQ24" s="6"/>
-      <c r="BR24" s="6"/>
-      <c r="BS24" s="6"/>
-      <c r="BT24" s="6"/>
-      <c r="BU24" s="6"/>
-      <c r="BV24" s="6"/>
-      <c r="BW24" s="6"/>
-      <c r="BX24" s="6"/>
-      <c r="BY24" s="6"/>
-      <c r="BZ24" s="6"/>
-      <c r="CA24" s="6"/>
-      <c r="CB24" s="6"/>
-      <c r="CC24" s="6"/>
-      <c r="CD24" s="6"/>
-      <c r="CE24" s="6"/>
-      <c r="CF24" s="6"/>
-      <c r="CG24" s="6"/>
-      <c r="CH24" s="6"/>
-      <c r="CI24" s="6"/>
-      <c r="CJ24" s="6"/>
-      <c r="CK24" s="6"/>
-      <c r="CL24" s="6"/>
-      <c r="CM24" s="6"/>
-      <c r="CN24" s="6"/>
+      <c r="BL24" s="7"/>
+      <c r="BM24" s="7"/>
+      <c r="BN24" s="7"/>
+      <c r="BO24" s="7"/>
+      <c r="BP24" s="7"/>
+      <c r="BQ24" s="7">
+        <v>25</v>
+      </c>
+      <c r="BR24" s="7"/>
+      <c r="BS24" s="7"/>
+      <c r="BT24" s="7"/>
+      <c r="BU24" s="7"/>
+      <c r="BV24" s="7"/>
+      <c r="BW24" s="7"/>
+      <c r="BX24" s="7"/>
+      <c r="BY24" s="7"/>
+      <c r="BZ24" s="7"/>
+      <c r="CA24" s="7"/>
+      <c r="CB24" s="7"/>
+      <c r="CC24" s="7"/>
+      <c r="CD24" s="7"/>
+      <c r="CE24" s="7"/>
+      <c r="CF24" s="7"/>
+      <c r="CG24" s="7"/>
+      <c r="CH24" s="7"/>
+      <c r="CI24" s="7"/>
+      <c r="CJ24" s="7"/>
+      <c r="CK24" s="7"/>
+      <c r="CL24" s="7"/>
+      <c r="CM24" s="7"/>
+      <c r="CN24" s="7"/>
     </row>
     <row r="25" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="7">
-        <v>20</v>
-      </c>
+      <c r="E25" s="7"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="7">
-        <v>40</v>
-      </c>
+      <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
-      <c r="L25" s="7">
-        <v>3</v>
-      </c>
+      <c r="L25" s="7"/>
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
@@ -4100,14 +4106,10 @@
       <c r="AB25" s="7"/>
       <c r="AC25" s="7"/>
       <c r="AD25" s="7"/>
-      <c r="AE25" s="7">
-        <v>40</v>
-      </c>
+      <c r="AE25" s="7"/>
       <c r="AF25" s="7"/>
       <c r="AG25" s="7"/>
-      <c r="AH25" s="7">
-        <v>0.1</v>
-      </c>
+      <c r="AH25" s="7"/>
       <c r="AI25" s="7"/>
       <c r="AJ25" s="7"/>
       <c r="AK25" s="7"/>
@@ -4119,9 +4121,7 @@
       <c r="AQ25" s="7"/>
       <c r="AR25" s="7"/>
       <c r="AS25" s="7"/>
-      <c r="AT25" s="7">
-        <v>5</v>
-      </c>
+      <c r="AT25" s="7"/>
       <c r="AU25" s="7"/>
       <c r="AV25" s="7"/>
       <c r="AW25" s="7"/>
@@ -4138,18 +4138,18 @@
       <c r="BH25" s="7"/>
       <c r="BI25" s="7"/>
       <c r="BJ25" s="7"/>
-      <c r="BK25" s="7">
-        <v>25</v>
-      </c>
+      <c r="BK25" s="7"/>
       <c r="BL25" s="7"/>
-      <c r="BM25" s="7"/>
-      <c r="BN25" s="7"/>
-      <c r="BO25" s="7"/>
-      <c r="BP25" s="7"/>
-      <c r="BQ25" s="7">
-        <v>25</v>
-      </c>
-      <c r="BR25" s="7"/>
+      <c r="BM25" s="14">
+        <v>10</v>
+      </c>
+      <c r="BN25" s="14"/>
+      <c r="BO25" s="14"/>
+      <c r="BP25" s="14"/>
+      <c r="BQ25" s="14"/>
+      <c r="BR25" s="14">
+        <v>5</v>
+      </c>
       <c r="BS25" s="7"/>
       <c r="BT25" s="7"/>
       <c r="BU25" s="7"/>
@@ -4175,10 +4175,10 @@
     </row>
     <row r="26" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -4186,7 +4186,9 @@
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="I26" s="7">
+        <v>2</v>
+      </c>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
@@ -4203,7 +4205,9 @@
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
-      <c r="Z26" s="7"/>
+      <c r="Z26" s="7">
+        <v>25</v>
+      </c>
       <c r="AA26" s="7"/>
       <c r="AB26" s="7"/>
       <c r="AC26" s="7"/>
@@ -4242,16 +4246,12 @@
       <c r="BJ26" s="7"/>
       <c r="BK26" s="7"/>
       <c r="BL26" s="7"/>
-      <c r="BM26" s="14">
-        <v>10</v>
-      </c>
-      <c r="BN26" s="14"/>
-      <c r="BO26" s="14"/>
-      <c r="BP26" s="14"/>
-      <c r="BQ26" s="14"/>
-      <c r="BR26" s="14">
-        <v>5</v>
-      </c>
+      <c r="BM26" s="7"/>
+      <c r="BN26" s="7"/>
+      <c r="BO26" s="7"/>
+      <c r="BP26" s="7"/>
+      <c r="BQ26" s="7"/>
+      <c r="BR26" s="7"/>
       <c r="BS26" s="7"/>
       <c r="BT26" s="7"/>
       <c r="BU26" s="7"/>
@@ -4270,17 +4270,17 @@
       <c r="CH26" s="7"/>
       <c r="CI26" s="7"/>
       <c r="CJ26" s="7"/>
-      <c r="CK26" s="7"/>
+      <c r="CK26" s="2"/>
       <c r="CL26" s="7"/>
       <c r="CM26" s="7"/>
       <c r="CN26" s="7"/>
     </row>
     <row r="27" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>127</v>
+        <v>27</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -4288,9 +4288,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
-      <c r="I27" s="7">
-        <v>2</v>
-      </c>
+      <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
@@ -4307,9 +4305,7 @@
       <c r="W27" s="7"/>
       <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
-      <c r="Z27" s="7">
-        <v>25</v>
-      </c>
+      <c r="Z27" s="7"/>
       <c r="AA27" s="7"/>
       <c r="AB27" s="7"/>
       <c r="AC27" s="7"/>
@@ -4372,17 +4368,19 @@
       <c r="CH27" s="7"/>
       <c r="CI27" s="7"/>
       <c r="CJ27" s="7"/>
-      <c r="CK27" s="2"/>
+      <c r="CK27" s="14">
+        <v>55</v>
+      </c>
       <c r="CL27" s="7"/>
       <c r="CM27" s="7"/>
       <c r="CN27" s="7"/>
     </row>
     <row r="28" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -4401,7 +4399,9 @@
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
       <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
+      <c r="T28" s="7">
+        <v>0.5</v>
+      </c>
       <c r="U28" s="7"/>
       <c r="V28" s="7"/>
       <c r="W28" s="7"/>
@@ -4414,7 +4414,9 @@
       <c r="AD28" s="7"/>
       <c r="AE28" s="7"/>
       <c r="AF28" s="7"/>
-      <c r="AG28" s="7"/>
+      <c r="AG28" s="7">
+        <v>0.2</v>
+      </c>
       <c r="AH28" s="7"/>
       <c r="AI28" s="7"/>
       <c r="AJ28" s="7"/>
@@ -4452,7 +4454,9 @@
       <c r="BP28" s="7"/>
       <c r="BQ28" s="7"/>
       <c r="BR28" s="7"/>
-      <c r="BS28" s="7"/>
+      <c r="BS28" s="7">
+        <v>10</v>
+      </c>
       <c r="BT28" s="7"/>
       <c r="BU28" s="7"/>
       <c r="BV28" s="7"/>
@@ -4470,19 +4474,17 @@
       <c r="CH28" s="7"/>
       <c r="CI28" s="7"/>
       <c r="CJ28" s="7"/>
-      <c r="CK28" s="14">
-        <v>55</v>
-      </c>
+      <c r="CK28" s="7"/>
       <c r="CL28" s="7"/>
       <c r="CM28" s="7"/>
       <c r="CN28" s="7"/>
     </row>
     <row r="29" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -4496,14 +4498,14 @@
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
+      <c r="O29" s="7">
+        <v>35</v>
+      </c>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
       <c r="R29" s="7"/>
       <c r="S29" s="7"/>
-      <c r="T29" s="7">
-        <v>0.5</v>
-      </c>
+      <c r="T29" s="7"/>
       <c r="U29" s="7"/>
       <c r="V29" s="7"/>
       <c r="W29" s="7"/>
@@ -4516,9 +4518,7 @@
       <c r="AD29" s="7"/>
       <c r="AE29" s="7"/>
       <c r="AF29" s="7"/>
-      <c r="AG29" s="7">
-        <v>0.2</v>
-      </c>
+      <c r="AG29" s="7"/>
       <c r="AH29" s="7"/>
       <c r="AI29" s="7"/>
       <c r="AJ29" s="7"/>
@@ -4530,13 +4530,17 @@
       <c r="AP29" s="7"/>
       <c r="AQ29" s="7"/>
       <c r="AR29" s="7"/>
-      <c r="AS29" s="7"/>
+      <c r="AS29" s="7">
+        <v>4</v>
+      </c>
       <c r="AT29" s="7"/>
       <c r="AU29" s="7"/>
       <c r="AV29" s="7"/>
       <c r="AW29" s="7"/>
       <c r="AX29" s="7"/>
-      <c r="AY29" s="7"/>
+      <c r="AY29" s="14">
+        <v>35</v>
+      </c>
       <c r="AZ29" s="7"/>
       <c r="BA29" s="7"/>
       <c r="BB29" s="7"/>
@@ -4547,23 +4551,33 @@
       <c r="BG29" s="7"/>
       <c r="BH29" s="7"/>
       <c r="BI29" s="7"/>
-      <c r="BJ29" s="7"/>
+      <c r="BJ29" s="7">
+        <v>50</v>
+      </c>
       <c r="BK29" s="7"/>
-      <c r="BL29" s="7"/>
+      <c r="BL29" s="7">
+        <v>8</v>
+      </c>
       <c r="BM29" s="7"/>
-      <c r="BN29" s="7"/>
+      <c r="BN29" s="7">
+        <v>35</v>
+      </c>
       <c r="BO29" s="7"/>
       <c r="BP29" s="7"/>
       <c r="BQ29" s="7"/>
-      <c r="BR29" s="7"/>
-      <c r="BS29" s="7">
+      <c r="BR29" s="7">
+        <v>55</v>
+      </c>
+      <c r="BS29" s="7"/>
+      <c r="BT29" s="7">
         <v>10</v>
       </c>
-      <c r="BT29" s="7"/>
       <c r="BU29" s="7"/>
       <c r="BV29" s="7"/>
       <c r="BW29" s="7"/>
-      <c r="BX29" s="7"/>
+      <c r="BX29" s="7">
+        <v>20</v>
+      </c>
       <c r="BY29" s="7"/>
       <c r="BZ29" s="7"/>
       <c r="CA29" s="7"/>
@@ -4578,15 +4592,17 @@
       <c r="CJ29" s="7"/>
       <c r="CK29" s="7"/>
       <c r="CL29" s="7"/>
-      <c r="CM29" s="7"/>
+      <c r="CM29" s="7">
+        <v>15</v>
+      </c>
       <c r="CN29" s="7"/>
     </row>
     <row r="30" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -4600,9 +4616,7 @@
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
-      <c r="O30" s="7">
-        <v>35</v>
-      </c>
+      <c r="O30" s="7"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
       <c r="R30" s="7"/>
@@ -4632,17 +4646,13 @@
       <c r="AP30" s="7"/>
       <c r="AQ30" s="7"/>
       <c r="AR30" s="7"/>
-      <c r="AS30" s="7">
-        <v>4</v>
-      </c>
+      <c r="AS30" s="7"/>
       <c r="AT30" s="7"/>
       <c r="AU30" s="7"/>
       <c r="AV30" s="7"/>
       <c r="AW30" s="7"/>
       <c r="AX30" s="7"/>
-      <c r="AY30" s="14">
-        <v>35</v>
-      </c>
+      <c r="AY30" s="7"/>
       <c r="AZ30" s="7"/>
       <c r="BA30" s="7"/>
       <c r="BB30" s="7"/>
@@ -4653,40 +4663,40 @@
       <c r="BG30" s="7"/>
       <c r="BH30" s="7"/>
       <c r="BI30" s="7"/>
-      <c r="BJ30" s="7">
-        <v>50</v>
-      </c>
+      <c r="BJ30" s="7"/>
       <c r="BK30" s="7"/>
-      <c r="BL30" s="7">
-        <v>8</v>
-      </c>
+      <c r="BL30" s="7"/>
       <c r="BM30" s="7"/>
-      <c r="BN30" s="7">
-        <v>35</v>
-      </c>
+      <c r="BN30" s="7"/>
       <c r="BO30" s="7"/>
       <c r="BP30" s="7"/>
       <c r="BQ30" s="7"/>
-      <c r="BR30" s="7">
-        <v>55</v>
-      </c>
+      <c r="BR30" s="7"/>
       <c r="BS30" s="7"/>
-      <c r="BT30" s="7">
-        <v>10</v>
-      </c>
+      <c r="BT30" s="7"/>
       <c r="BU30" s="7"/>
       <c r="BV30" s="7"/>
-      <c r="BW30" s="7"/>
+      <c r="BW30" s="7">
+        <v>15</v>
+      </c>
       <c r="BX30" s="7">
-        <v>20</v>
-      </c>
-      <c r="BY30" s="7"/>
-      <c r="BZ30" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="BY30" s="7">
+        <v>5</v>
+      </c>
+      <c r="BZ30" s="7">
+        <v>10</v>
+      </c>
       <c r="CA30" s="7"/>
       <c r="CB30" s="7"/>
-      <c r="CC30" s="7"/>
+      <c r="CC30" s="7">
+        <v>8</v>
+      </c>
       <c r="CD30" s="7"/>
-      <c r="CE30" s="7"/>
+      <c r="CE30" s="7">
+        <v>5</v>
+      </c>
       <c r="CF30" s="7"/>
       <c r="CG30" s="7"/>
       <c r="CH30" s="7"/>
@@ -4694,786 +4704,316 @@
       <c r="CJ30" s="7"/>
       <c r="CK30" s="7"/>
       <c r="CL30" s="7"/>
-      <c r="CM30" s="7">
+      <c r="CM30" s="7"/>
+      <c r="CN30" s="7"/>
+    </row>
+    <row r="31" spans="1:108" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="10">
+        <v>3</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10">
+        <v>85</v>
+      </c>
+      <c r="G31" s="10">
+        <v>50.1</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10">
+        <v>6</v>
+      </c>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10">
+        <v>40</v>
+      </c>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10">
+        <v>20</v>
+      </c>
+      <c r="N31" s="10">
+        <v>40</v>
+      </c>
+      <c r="O31" s="13">
+        <v>31</v>
+      </c>
+      <c r="P31" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10">
+        <v>40</v>
+      </c>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10">
+        <v>44</v>
+      </c>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10">
+        <v>45</v>
+      </c>
+      <c r="X31" s="10"/>
+      <c r="Y31" s="10">
         <v>15</v>
       </c>
-      <c r="CN30" s="7"/>
-    </row>
-    <row r="31" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-      <c r="AA31" s="7"/>
-      <c r="AB31" s="7"/>
-      <c r="AC31" s="7"/>
-      <c r="AD31" s="7"/>
-      <c r="AE31" s="7"/>
-      <c r="AF31" s="7"/>
-      <c r="AG31" s="7"/>
-      <c r="AH31" s="7"/>
-      <c r="AI31" s="7"/>
-      <c r="AJ31" s="7"/>
-      <c r="AK31" s="7"/>
-      <c r="AL31" s="7"/>
-      <c r="AM31" s="7"/>
-      <c r="AN31" s="7"/>
-      <c r="AO31" s="7"/>
-      <c r="AP31" s="7"/>
-      <c r="AQ31" s="7"/>
-      <c r="AR31" s="7"/>
-      <c r="AS31" s="7"/>
-      <c r="AT31" s="7"/>
-      <c r="AU31" s="7"/>
-      <c r="AV31" s="7"/>
-      <c r="AW31" s="7"/>
-      <c r="AX31" s="7"/>
-      <c r="AY31" s="7"/>
-      <c r="AZ31" s="7"/>
-      <c r="BA31" s="7"/>
-      <c r="BB31" s="7"/>
-      <c r="BC31" s="7"/>
-      <c r="BD31" s="7"/>
-      <c r="BE31" s="7"/>
-      <c r="BF31" s="7"/>
-      <c r="BG31" s="7"/>
-      <c r="BH31" s="7"/>
-      <c r="BI31" s="7"/>
-      <c r="BJ31" s="7"/>
-      <c r="BK31" s="7"/>
-      <c r="BL31" s="7"/>
-      <c r="BM31" s="7"/>
-      <c r="BN31" s="7"/>
-      <c r="BO31" s="7"/>
-      <c r="BP31" s="7"/>
-      <c r="BQ31" s="7"/>
-      <c r="BR31" s="7"/>
-      <c r="BS31" s="7"/>
-      <c r="BT31" s="7"/>
-      <c r="BU31" s="7"/>
-      <c r="BV31" s="7"/>
-      <c r="BW31" s="7">
+      <c r="Z31" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="10"/>
+      <c r="AB31" s="10"/>
+      <c r="AC31" s="10"/>
+      <c r="AD31" s="10"/>
+      <c r="AE31" s="10"/>
+      <c r="AF31" s="10"/>
+      <c r="AG31" s="10"/>
+      <c r="AH31" s="10"/>
+      <c r="AI31" s="10"/>
+      <c r="AJ31" s="10">
+        <v>55</v>
+      </c>
+      <c r="AK31" s="10">
+        <v>1</v>
+      </c>
+      <c r="AL31" s="10"/>
+      <c r="AM31" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="AN31" s="10"/>
+      <c r="AO31" s="10">
+        <v>2</v>
+      </c>
+      <c r="AP31" s="10"/>
+      <c r="AQ31" s="10"/>
+      <c r="AR31" s="10">
+        <v>30</v>
+      </c>
+      <c r="AS31" s="10"/>
+      <c r="AT31" s="10"/>
+      <c r="AU31" s="10"/>
+      <c r="AV31" s="10"/>
+      <c r="AW31" s="10"/>
+      <c r="AX31" s="10"/>
+      <c r="AY31" s="10"/>
+      <c r="AZ31" s="10"/>
+      <c r="BA31" s="10"/>
+      <c r="BB31" s="10"/>
+      <c r="BC31" s="10"/>
+      <c r="BD31" s="10"/>
+      <c r="BE31" s="10"/>
+      <c r="BF31" s="10"/>
+      <c r="BG31" s="10"/>
+      <c r="BH31" s="10"/>
+      <c r="BI31" s="10"/>
+      <c r="BJ31" s="10"/>
+      <c r="BK31" s="10"/>
+      <c r="BL31" s="10">
+        <v>25</v>
+      </c>
+      <c r="BM31" s="5"/>
+      <c r="BN31" s="10"/>
+      <c r="BO31" s="10">
+        <v>2</v>
+      </c>
+      <c r="BP31" s="10"/>
+      <c r="BQ31" s="10"/>
+      <c r="BR31" s="5"/>
+      <c r="BS31" s="10">
         <v>15</v>
       </c>
-      <c r="BX31" s="7">
+      <c r="BT31" s="10"/>
+      <c r="BU31" s="10">
+        <v>20</v>
+      </c>
+      <c r="BV31" s="10"/>
+      <c r="BW31" s="10"/>
+      <c r="BX31" s="13">
+        <v>15</v>
+      </c>
+      <c r="BY31" s="10"/>
+      <c r="BZ31" s="10"/>
+      <c r="CA31" s="10"/>
+      <c r="CB31" s="10"/>
+      <c r="CC31" s="10"/>
+      <c r="CD31" s="10">
+        <v>20</v>
+      </c>
+      <c r="CE31" s="10">
+        <v>1</v>
+      </c>
+      <c r="CF31" s="10"/>
+      <c r="CG31" s="10">
         <v>10</v>
       </c>
-      <c r="BY31" s="7">
-        <v>5</v>
-      </c>
-      <c r="BZ31" s="7">
-        <v>10</v>
-      </c>
-      <c r="CA31" s="7"/>
-      <c r="CB31" s="7"/>
-      <c r="CC31" s="7">
-        <v>8</v>
-      </c>
-      <c r="CD31" s="7"/>
-      <c r="CE31" s="7">
-        <v>5</v>
-      </c>
-      <c r="CF31" s="7"/>
-      <c r="CG31" s="7"/>
-      <c r="CH31" s="7"/>
-      <c r="CI31" s="7"/>
-      <c r="CJ31" s="7"/>
-      <c r="CK31" s="7"/>
-      <c r="CL31" s="7"/>
-      <c r="CM31" s="7"/>
-      <c r="CN31" s="7"/>
-    </row>
-    <row r="32" spans="1:108" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="10">
-        <v>3</v>
-      </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10">
-        <v>85</v>
-      </c>
-      <c r="G32" s="10">
-        <v>50.1</v>
-      </c>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10">
-        <v>6</v>
-      </c>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10">
-        <v>40</v>
-      </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10">
-        <v>20</v>
-      </c>
-      <c r="N32" s="10">
-        <v>40</v>
-      </c>
-      <c r="O32" s="13">
-        <v>31</v>
-      </c>
-      <c r="P32" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="10">
-        <v>40</v>
-      </c>
-      <c r="S32" s="10"/>
-      <c r="T32" s="10">
-        <v>44</v>
-      </c>
-      <c r="U32" s="10"/>
-      <c r="V32" s="10"/>
-      <c r="W32" s="10">
-        <v>45</v>
-      </c>
-      <c r="X32" s="10"/>
-      <c r="Y32" s="10">
-        <v>15</v>
-      </c>
-      <c r="Z32" s="10">
-        <v>1</v>
-      </c>
-      <c r="AA32" s="10"/>
-      <c r="AB32" s="10"/>
-      <c r="AC32" s="10"/>
-      <c r="AD32" s="10"/>
-      <c r="AE32" s="10"/>
-      <c r="AF32" s="10"/>
-      <c r="AG32" s="10"/>
-      <c r="AH32" s="10"/>
-      <c r="AI32" s="10"/>
-      <c r="AJ32" s="10">
-        <v>55</v>
-      </c>
-      <c r="AK32" s="10">
-        <v>1</v>
-      </c>
-      <c r="AL32" s="10"/>
-      <c r="AM32" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="AN32" s="10"/>
-      <c r="AO32" s="10">
-        <v>2</v>
-      </c>
-      <c r="AP32" s="10"/>
-      <c r="AQ32" s="10"/>
-      <c r="AR32" s="10">
+      <c r="CH31" s="10"/>
+      <c r="CI31" s="10">
         <v>30</v>
       </c>
-      <c r="AS32" s="10"/>
-      <c r="AT32" s="10"/>
-      <c r="AU32" s="10"/>
-      <c r="AV32" s="10"/>
-      <c r="AW32" s="10"/>
-      <c r="AX32" s="10"/>
-      <c r="AY32" s="10"/>
-      <c r="AZ32" s="10"/>
-      <c r="BA32" s="10"/>
-      <c r="BB32" s="10"/>
-      <c r="BC32" s="10"/>
-      <c r="BD32" s="10"/>
-      <c r="BE32" s="10"/>
-      <c r="BF32" s="10"/>
-      <c r="BG32" s="10"/>
-      <c r="BH32" s="10"/>
-      <c r="BI32" s="10"/>
-      <c r="BJ32" s="10"/>
-      <c r="BK32" s="10"/>
-      <c r="BL32" s="10">
-        <v>25</v>
-      </c>
-      <c r="BM32" s="5"/>
-      <c r="BN32" s="10"/>
-      <c r="BO32" s="10">
-        <v>2</v>
-      </c>
-      <c r="BP32" s="10"/>
-      <c r="BQ32" s="10"/>
-      <c r="BR32" s="5"/>
-      <c r="BS32" s="10">
-        <v>15</v>
-      </c>
-      <c r="BT32" s="10"/>
-      <c r="BU32" s="10">
-        <v>20</v>
-      </c>
-      <c r="BV32" s="10"/>
-      <c r="BW32" s="10"/>
-      <c r="BX32" s="13">
-        <v>15</v>
-      </c>
-      <c r="BY32" s="10"/>
-      <c r="BZ32" s="10"/>
-      <c r="CA32" s="10"/>
-      <c r="CB32" s="10"/>
-      <c r="CC32" s="10"/>
-      <c r="CD32" s="10">
-        <v>20</v>
-      </c>
-      <c r="CE32" s="10">
-        <v>1</v>
-      </c>
-      <c r="CF32" s="10"/>
-      <c r="CG32" s="10">
-        <v>10</v>
-      </c>
-      <c r="CH32" s="10"/>
-      <c r="CI32" s="10">
-        <v>30</v>
-      </c>
-      <c r="CJ32" s="10"/>
-      <c r="CK32" s="10"/>
-      <c r="CL32" s="10"/>
-      <c r="CM32" s="10"/>
-      <c r="CN32" s="10"/>
-      <c r="CO32" s="11"/>
-      <c r="CP32" s="11"/>
-    </row>
-    <row r="33" spans="1:92" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="6">
-        <f>SUM(C2:C32)</f>
-        <v>95</v>
-      </c>
-      <c r="D33" s="6">
-        <f>SUM(D2:D32)</f>
-        <v>123.1</v>
-      </c>
-      <c r="E33" s="6">
-        <f>SUM(E2:E32)</f>
-        <v>110.1</v>
-      </c>
-      <c r="F33" s="6">
-        <f>SUM(F2:F32)</f>
-        <v>120</v>
-      </c>
-      <c r="G33" s="6">
-        <f>SUM(G2:G32)</f>
-        <v>135.30000000000001</v>
-      </c>
-      <c r="H33" s="6">
-        <f>SUM(H2:H32)</f>
-        <v>47.1</v>
-      </c>
-      <c r="I33" s="6">
-        <f>SUM(I2:I32)</f>
-        <v>118</v>
-      </c>
-      <c r="J33" s="6">
-        <f>SUM(J2:J32)</f>
-        <v>99.199999999999989</v>
-      </c>
-      <c r="K33" s="6">
-        <f>SUM(K2:K32)</f>
-        <v>110.5</v>
-      </c>
-      <c r="L33" s="6">
-        <f>SUM(L2:L32)</f>
-        <v>78.099999999999994</v>
-      </c>
-      <c r="M33" s="6">
-        <f>SUM(M2:M32)</f>
-        <v>115</v>
-      </c>
-      <c r="N33" s="6">
-        <f>SUM(N2:N32)</f>
-        <v>148</v>
-      </c>
-      <c r="O33" s="6">
-        <f>SUM(O2:O32)</f>
-        <v>105.2</v>
-      </c>
-      <c r="P33" s="6">
-        <f>SUM(P2:P32)</f>
-        <v>94.6</v>
-      </c>
-      <c r="Q33" s="6">
-        <f>SUM(Q2:Q32)</f>
-        <v>95.1</v>
-      </c>
-      <c r="R33" s="6">
-        <f>SUM(R2:R32)</f>
-        <v>100</v>
-      </c>
-      <c r="S33" s="6">
-        <f>SUM(S2:S32)</f>
-        <v>70</v>
-      </c>
-      <c r="T33" s="6">
-        <f>SUM(T2:T32)</f>
-        <v>80</v>
-      </c>
-      <c r="U33" s="6">
-        <f>SUM(U2:U32)</f>
-        <v>98.1</v>
-      </c>
-      <c r="V33" s="6">
-        <f>SUM(V2:V32)</f>
-        <v>75</v>
-      </c>
-      <c r="W33" s="6">
-        <f>SUM(W2:W32)</f>
-        <v>79</v>
-      </c>
-      <c r="X33" s="6">
-        <f>SUM(X2:X32)</f>
-        <v>100</v>
-      </c>
-      <c r="Y33" s="6">
-        <f>SUM(Y2:Y32)</f>
-        <v>96</v>
-      </c>
-      <c r="Z33" s="6">
-        <f>SUM(Z2:Z32)</f>
-        <v>55</v>
-      </c>
-      <c r="AA33" s="6">
-        <f>SUM(AA2:AA32)</f>
-        <v>105</v>
-      </c>
-      <c r="AB33" s="6">
-        <f>SUM(AB2:AB32)</f>
-        <v>98</v>
-      </c>
-      <c r="AC33" s="6">
-        <f>SUM(AC2:AC32)</f>
-        <v>80</v>
-      </c>
-      <c r="AD33" s="6">
-        <f>SUM(AD2:AD32)</f>
-        <v>65</v>
-      </c>
-      <c r="AE33" s="6">
-        <f>SUM(AE2:AE32)</f>
-        <v>109</v>
-      </c>
-      <c r="AF33" s="6">
-        <f>SUM(AF2:AF32)</f>
-        <v>110</v>
-      </c>
-      <c r="AG33" s="6">
-        <f>SUM(AG2:AG32)</f>
-        <v>92.2</v>
-      </c>
-      <c r="AH33" s="6">
-        <f>SUM(AH2:AH32)</f>
-        <v>97.1</v>
-      </c>
-      <c r="AI33" s="6">
-        <f t="shared" ref="AI33:BN33" si="0">SUM(AI2:AI32)</f>
-        <v>100.1</v>
-      </c>
-      <c r="AJ33" s="6">
-        <f t="shared" si="0"/>
-        <v>102.5</v>
-      </c>
-      <c r="AK33" s="6">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="AL33" s="6">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="AM33" s="6">
-        <f t="shared" si="0"/>
-        <v>101.9</v>
-      </c>
-      <c r="AN33" s="6">
-        <f t="shared" si="0"/>
-        <v>115</v>
-      </c>
-      <c r="AO33" s="6">
-        <f t="shared" si="0"/>
-        <v>106</v>
-      </c>
-      <c r="AP33" s="6">
-        <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-      <c r="AQ33" s="6">
-        <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-      <c r="AR33" s="6">
-        <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-      <c r="AS33" s="6">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="AT33" s="6">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="AU33" s="6">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="AV33" s="6">
-        <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-      <c r="AW33" s="6">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="AX33" s="6">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="AY33" s="6">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-      <c r="AZ33" s="6">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="BA33" s="6">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
-      <c r="BB33" s="6">
-        <f t="shared" si="0"/>
-        <v>91</v>
-      </c>
-      <c r="BC33" s="6">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="BD33" s="6">
-        <f t="shared" si="0"/>
-        <v>90.2</v>
-      </c>
-      <c r="BE33" s="6">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="BF33" s="6">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="BG33" s="6">
-        <f t="shared" si="0"/>
-        <v>93</v>
-      </c>
-      <c r="BH33" s="6">
-        <f t="shared" si="0"/>
-        <v>96.3</v>
-      </c>
-      <c r="BI33" s="6">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="BJ33" s="6">
-        <f t="shared" si="0"/>
-        <v>60.5</v>
-      </c>
-      <c r="BK33" s="6">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="BL33" s="6">
-        <f t="shared" si="0"/>
-        <v>93</v>
-      </c>
-      <c r="BM33" s="6">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-      <c r="BN33" s="6">
-        <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="BO33" s="6">
-        <f>SUM(BO2:BO32)</f>
-        <v>132</v>
-      </c>
-      <c r="BP33" s="6">
-        <f>SUM(BP2:BP32)</f>
-        <v>106.2</v>
-      </c>
-      <c r="BQ33" s="6">
-        <f>SUM(BQ2:BQ32)</f>
-        <v>50.5</v>
-      </c>
-      <c r="BR33" s="6">
-        <f>SUM(BR2:BR32)</f>
-        <v>75</v>
-      </c>
-      <c r="BS33" s="6">
-        <f>SUM(BS2:BS32)</f>
-        <v>46</v>
-      </c>
-      <c r="BT33" s="6">
-        <f>SUM(BT2:BT32)</f>
-        <v>74</v>
-      </c>
-      <c r="BU33" s="6">
-        <f>SUM(BU2:BU32)</f>
-        <v>74</v>
-      </c>
-      <c r="BV33" s="6">
-        <f>SUM(BV2:BV32)</f>
-        <v>115</v>
-      </c>
-      <c r="BW33" s="6">
-        <f>SUM(BW2:BW32)</f>
-        <v>33</v>
-      </c>
-      <c r="BX33" s="6">
-        <f>SUM(BX2:BX32)</f>
-        <v>76</v>
-      </c>
-      <c r="BY33" s="6">
-        <f>SUM(BY2:BY32)</f>
-        <v>61</v>
-      </c>
-      <c r="BZ33" s="6">
-        <f>SUM(BZ2:BZ32)</f>
-        <v>11.5</v>
-      </c>
-      <c r="CA33" s="6">
-        <f>SUM(CA2:CA32)</f>
-        <v>74</v>
-      </c>
-      <c r="CB33" s="6">
-        <f>SUM(CB2:CB32)</f>
-        <v>105.5</v>
-      </c>
-      <c r="CC33" s="6">
-        <f>SUM(CC2:CC32)</f>
-        <v>69</v>
-      </c>
-      <c r="CD33" s="6">
-        <f>SUM(CD2:CD32)</f>
-        <v>101.5</v>
-      </c>
-      <c r="CE33" s="6">
-        <f>SUM(CE2:CE32)</f>
-        <v>96</v>
-      </c>
-      <c r="CF33" s="6">
-        <f>SUM(CF2:CF32)</f>
-        <v>100</v>
-      </c>
-      <c r="CG33" s="6">
-        <f>SUM(CG2:CG32)</f>
-        <v>81</v>
-      </c>
-      <c r="CH33" s="6">
-        <f>SUM(CH2:CH32)</f>
-        <v>98</v>
-      </c>
-      <c r="CI33" s="6">
-        <f>SUM(CI2:CI32)</f>
-        <v>95</v>
-      </c>
-      <c r="CJ33" s="6">
-        <f>SUM(CJ2:CJ32)</f>
-        <v>70</v>
-      </c>
-      <c r="CK33" s="6">
-        <f>SUM(CK2:CK32)</f>
-        <v>55</v>
-      </c>
-      <c r="CL33" s="6">
-        <f>SUM(CL2:CL32)</f>
-        <v>89</v>
-      </c>
-      <c r="CM33" s="6">
-        <f>SUM(CM2:CM32)</f>
-        <v>47</v>
-      </c>
-      <c r="CN33" s="6">
-        <f>SUM(CN2:CN32)</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:92" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
-      <c r="X34" s="2"/>
-      <c r="Y34" s="2"/>
-      <c r="Z34" s="2"/>
-      <c r="AA34" s="2"/>
-      <c r="AB34" s="2"/>
-      <c r="AC34" s="2"/>
-      <c r="AD34" s="2"/>
-      <c r="AE34" s="2"/>
-      <c r="AF34" s="2"/>
-      <c r="AG34" s="2"/>
-      <c r="AH34" s="2"/>
-      <c r="AI34" s="2"/>
-      <c r="AJ34" s="2"/>
-      <c r="AK34" s="2"/>
-      <c r="AL34" s="2"/>
-      <c r="AM34" s="2"/>
-      <c r="AN34" s="2"/>
-      <c r="AO34" s="2"/>
-      <c r="AP34" s="2"/>
-      <c r="AQ34" s="2"/>
-      <c r="AR34" s="2"/>
-      <c r="AS34" s="2"/>
-      <c r="AT34" s="2"/>
-      <c r="AU34" s="2"/>
-      <c r="AV34" s="2"/>
-      <c r="AW34" s="2"/>
-      <c r="AX34" s="2"/>
-      <c r="AY34" s="2"/>
-      <c r="AZ34" s="2"/>
-      <c r="BA34" s="2"/>
-      <c r="BB34" s="2"/>
-      <c r="BC34" s="2"/>
-      <c r="BD34" s="2"/>
-      <c r="BE34" s="2"/>
-      <c r="BF34" s="2"/>
-      <c r="BG34" s="2"/>
-      <c r="BH34" s="2"/>
-      <c r="BI34" s="2"/>
-      <c r="BJ34" s="2"/>
-      <c r="BK34" s="2"/>
-      <c r="BL34" s="2"/>
-      <c r="BM34" s="2"/>
-      <c r="BN34" s="2"/>
-      <c r="BO34" s="2"/>
-      <c r="BP34" s="2"/>
-      <c r="BQ34" s="2"/>
-      <c r="BR34" s="2"/>
-      <c r="BS34" s="2"/>
-      <c r="BT34" s="2"/>
-      <c r="BU34" s="2"/>
-      <c r="BV34" s="2"/>
-      <c r="BW34" s="2"/>
-      <c r="BX34" s="2"/>
-      <c r="BY34" s="2"/>
-      <c r="BZ34" s="2"/>
-      <c r="CA34" s="2"/>
-      <c r="CB34" s="2"/>
-      <c r="CC34" s="2"/>
-      <c r="CD34" s="2"/>
-      <c r="CE34" s="2"/>
-      <c r="CF34" s="2"/>
-      <c r="CG34" s="2"/>
-      <c r="CH34" s="2"/>
-      <c r="CI34" s="2"/>
-      <c r="CJ34" s="2"/>
-      <c r="CK34" s="2"/>
-      <c r="CL34" s="2"/>
-      <c r="CM34" s="2"/>
-      <c r="CN34" s="2"/>
-    </row>
-    <row r="36" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="CJ31" s="10"/>
+      <c r="CK31" s="10"/>
+      <c r="CL31" s="10"/>
+      <c r="CM31" s="10"/>
+      <c r="CN31" s="10"/>
+      <c r="CO31" s="11"/>
+      <c r="CP31" s="11"/>
+    </row>
+    <row r="32" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="2"/>
+      <c r="AG32" s="2"/>
+      <c r="AH32" s="2"/>
+      <c r="AI32" s="2"/>
+      <c r="AJ32" s="2"/>
+      <c r="AK32" s="2"/>
+      <c r="AL32" s="2"/>
+      <c r="AM32" s="2"/>
+      <c r="AN32" s="2"/>
+      <c r="AO32" s="2"/>
+      <c r="AP32" s="2"/>
+      <c r="AQ32" s="2"/>
+      <c r="AR32" s="2"/>
+      <c r="AS32" s="2"/>
+      <c r="AT32" s="2"/>
+      <c r="AU32" s="2"/>
+      <c r="AV32" s="2"/>
+      <c r="AW32" s="2"/>
+      <c r="AX32" s="2"/>
+      <c r="AY32" s="2"/>
+      <c r="AZ32" s="2"/>
+      <c r="BA32" s="2"/>
+      <c r="BB32" s="2"/>
+      <c r="BC32" s="2"/>
+      <c r="BD32" s="2"/>
+      <c r="BE32" s="2"/>
+      <c r="BF32" s="2"/>
+      <c r="BG32" s="2"/>
+      <c r="BH32" s="2"/>
+      <c r="BI32" s="2"/>
+      <c r="BJ32" s="2"/>
+      <c r="BK32" s="2"/>
+      <c r="BL32" s="2"/>
+      <c r="BM32" s="2"/>
+      <c r="BN32" s="2"/>
+      <c r="BO32" s="2"/>
+      <c r="BP32" s="2"/>
+      <c r="BQ32" s="2"/>
+      <c r="BR32" s="2"/>
+      <c r="BS32" s="2"/>
+      <c r="BT32" s="2"/>
+      <c r="BU32" s="2"/>
+      <c r="BV32" s="2"/>
+      <c r="BW32" s="2"/>
+      <c r="BX32" s="2"/>
+      <c r="BY32" s="2"/>
+      <c r="BZ32" s="2"/>
+      <c r="CA32" s="2"/>
+      <c r="CB32" s="2"/>
+      <c r="CC32" s="2"/>
+      <c r="CD32" s="2"/>
+      <c r="CE32" s="2"/>
+      <c r="CF32" s="2"/>
+      <c r="CG32" s="2"/>
+      <c r="CH32" s="2"/>
+      <c r="CI32" s="2"/>
+      <c r="CJ32" s="2"/>
+      <c r="CK32" s="2"/>
+      <c r="CL32" s="2"/>
+      <c r="CM32" s="2"/>
+      <c r="CN32" s="2"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="15"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="15"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="15"/>
     </row>
-    <row r="37" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="15"/>
     </row>
-    <row r="38" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="15"/>
     </row>
-    <row r="39" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="15"/>
     </row>
-    <row r="40" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="15"/>
     </row>
-    <row r="41" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="15"/>
     </row>
-    <row r="42" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="15"/>
     </row>
-    <row r="43" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="15"/>
     </row>
-    <row r="44" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="15"/>
     </row>
-    <row r="45" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="15"/>
     </row>
-    <row r="46" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="15"/>
     </row>
-    <row r="47" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="15"/>
     </row>
-    <row r="48" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="15"/>
     </row>
@@ -6116,14 +5656,6 @@
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="15"/>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="1"/>
-      <c r="B209" s="15"/>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="1"/>
-      <c r="B210" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added script, renamed others
</commit_message>
<xml_diff>
--- a/2.Data/VegetationData.xlsx
+++ b/2.Data/VegetationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/evert_sprockel_wur_nl/Documents/5.Wageningen/7.Thesis/7.DataAnalysis/TsoKarVegetationDataAnalysisR/2.Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="634" documentId="8_{872A76ED-DD01-460B-A727-DB46B93C166B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D483D43-F33C-47F4-8D78-C509177E7954}"/>
+  <xr:revisionPtr revIDLastSave="645" documentId="8_{872A76ED-DD01-460B-A727-DB46B93C166B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{107132E7-3CC6-4EB0-BE41-E2407900FF42}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DACF362B-6137-4498-953D-1E748F44EEF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DACF362B-6137-4498-953D-1E748F44EEF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -614,6 +614,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -936,10 +940,10 @@
   <dimension ref="A1:DD208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BP8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U16" sqref="U16"/>
+      <selection pane="bottomRight" activeCell="CO35" sqref="A35:CO38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4983,7 +4987,7 @@
       <c r="CM32" s="1"/>
       <c r="CN32" s="1"/>
     </row>
-    <row r="33" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:93" x14ac:dyDescent="0.25">
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
@@ -5075,63 +5079,245 @@
       <c r="CM33" s="14"/>
       <c r="CN33" s="14"/>
     </row>
-    <row r="34" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="14"/>
+      <c r="X36" s="14"/>
+      <c r="Y36" s="14"/>
+      <c r="Z36" s="14"/>
+      <c r="AA36" s="14"/>
+      <c r="AB36" s="14"/>
+      <c r="AC36" s="14"/>
+      <c r="AD36" s="14"/>
+      <c r="AE36" s="14"/>
+      <c r="AF36" s="14"/>
+      <c r="AG36" s="14"/>
+      <c r="AH36" s="14"/>
+      <c r="AI36" s="14"/>
+      <c r="AJ36" s="14"/>
+      <c r="AK36" s="14"/>
+      <c r="AL36" s="14"/>
+      <c r="AM36" s="14"/>
+      <c r="AN36" s="14"/>
+      <c r="AO36" s="14"/>
+      <c r="AP36" s="14"/>
+      <c r="AQ36" s="14"/>
+      <c r="AR36" s="14"/>
+      <c r="AS36" s="14"/>
+      <c r="AT36" s="14"/>
+      <c r="AU36" s="14"/>
+      <c r="AV36" s="14"/>
+      <c r="AW36" s="14"/>
+      <c r="AX36" s="14"/>
+      <c r="AY36" s="14"/>
+      <c r="AZ36" s="14"/>
+      <c r="BA36" s="14"/>
+      <c r="BB36" s="14"/>
+      <c r="BC36" s="14"/>
+      <c r="BD36" s="14"/>
+      <c r="BE36" s="14"/>
+      <c r="BF36" s="14"/>
+      <c r="BG36" s="14"/>
+      <c r="BH36" s="14"/>
+      <c r="BI36" s="14"/>
+      <c r="BJ36" s="14"/>
+      <c r="BK36" s="14"/>
+      <c r="BL36" s="14"/>
+      <c r="BM36" s="14"/>
+      <c r="BN36" s="14"/>
+      <c r="BO36" s="14"/>
+      <c r="BP36" s="14"/>
+      <c r="BQ36" s="14"/>
+      <c r="BR36" s="14"/>
+      <c r="BS36" s="14"/>
+      <c r="BT36" s="14"/>
+      <c r="BU36" s="14"/>
+      <c r="BV36" s="14"/>
+      <c r="BW36" s="14"/>
+      <c r="BX36" s="14"/>
+      <c r="BY36" s="14"/>
+      <c r="BZ36" s="14"/>
+      <c r="CA36" s="14"/>
+      <c r="CB36" s="14"/>
+      <c r="CC36" s="14"/>
+      <c r="CD36" s="14"/>
+      <c r="CE36" s="14"/>
+      <c r="CF36" s="14"/>
+      <c r="CG36" s="14"/>
+      <c r="CH36" s="14"/>
+      <c r="CI36" s="14"/>
+      <c r="CJ36" s="14"/>
+      <c r="CK36" s="14"/>
+      <c r="CL36" s="14"/>
+      <c r="CM36" s="14"/>
+      <c r="CN36" s="14"/>
+      <c r="CO36" s="14"/>
+    </row>
+    <row r="37" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="6"/>
-    </row>
-    <row r="38" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="14"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="14"/>
+      <c r="AF37" s="14"/>
+      <c r="AG37" s="14"/>
+      <c r="AH37" s="14"/>
+      <c r="AI37" s="14"/>
+      <c r="AJ37" s="14"/>
+      <c r="AK37" s="14"/>
+      <c r="AL37" s="14"/>
+      <c r="AM37" s="14"/>
+      <c r="AN37" s="14"/>
+      <c r="AO37" s="14"/>
+      <c r="AP37" s="14"/>
+      <c r="AQ37" s="14"/>
+      <c r="AR37" s="14"/>
+      <c r="AS37" s="14"/>
+      <c r="AT37" s="14"/>
+      <c r="AU37" s="14"/>
+      <c r="AV37" s="14"/>
+      <c r="AW37" s="14"/>
+      <c r="AX37" s="14"/>
+      <c r="AY37" s="14"/>
+      <c r="AZ37" s="14"/>
+      <c r="BA37" s="14"/>
+      <c r="BB37" s="14"/>
+      <c r="BC37" s="14"/>
+      <c r="BD37" s="14"/>
+      <c r="BE37" s="14"/>
+      <c r="BF37" s="14"/>
+      <c r="BG37" s="14"/>
+      <c r="BH37" s="14"/>
+      <c r="BI37" s="14"/>
+      <c r="BJ37" s="14"/>
+      <c r="BK37" s="14"/>
+      <c r="BL37" s="14"/>
+      <c r="BM37" s="14"/>
+      <c r="BN37" s="14"/>
+      <c r="BO37" s="14"/>
+      <c r="BP37" s="14"/>
+      <c r="BQ37" s="14"/>
+      <c r="BR37" s="14"/>
+      <c r="BS37" s="14"/>
+      <c r="BT37" s="14"/>
+      <c r="BU37" s="14"/>
+      <c r="BV37" s="14"/>
+      <c r="BW37" s="14"/>
+      <c r="BX37" s="14"/>
+      <c r="BY37" s="14"/>
+      <c r="BZ37" s="14"/>
+      <c r="CA37" s="14"/>
+      <c r="CB37" s="14"/>
+      <c r="CC37" s="14"/>
+      <c r="CD37" s="14"/>
+      <c r="CE37" s="14"/>
+      <c r="CF37" s="14"/>
+      <c r="CG37" s="14"/>
+      <c r="CH37" s="14"/>
+      <c r="CI37" s="14"/>
+      <c r="CJ37" s="14"/>
+      <c r="CK37" s="14"/>
+      <c r="CL37" s="14"/>
+      <c r="CM37" s="14"/>
+      <c r="CN37" s="14"/>
+      <c r="CO37" s="14"/>
+    </row>
+    <row r="38" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
       <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="6"/>
     </row>
-    <row r="41" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
       <c r="B41" s="6"/>
     </row>
-    <row r="42" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="6"/>
     </row>
-    <row r="43" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
       <c r="B43" s="6"/>
     </row>
-    <row r="44" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="6"/>
     </row>
-    <row r="45" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="6"/>
     </row>
-    <row r="46" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="6"/>
     </row>
-    <row r="47" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="6"/>
     </row>
-    <row r="48" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="6"/>
     </row>

</xml_diff>

<commit_message>
Added a few scripts
</commit_message>
<xml_diff>
--- a/2.Data/VegetationData.xlsx
+++ b/2.Data/VegetationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/evert_sprockel_wur_nl/Documents/5.Wageningen/7.Thesis/7.DataAnalysis/TsoKarVegetationDataAnalysisR/2.Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="645" documentId="8_{872A76ED-DD01-460B-A727-DB46B93C166B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{107132E7-3CC6-4EB0-BE41-E2407900FF42}"/>
+  <xr:revisionPtr revIDLastSave="649" documentId="8_{872A76ED-DD01-460B-A727-DB46B93C166B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69C2E59A-4D90-4497-A95F-520246C8D3AE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DACF362B-6137-4498-953D-1E748F44EEF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DACF362B-6137-4498-953D-1E748F44EEF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="129">
   <si>
     <t>Argentina anserina</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Knorringia pamirica</t>
   </si>
   <si>
-    <t>Lomatogonium branchyantherum</t>
-  </si>
-  <si>
     <t>Pedicularis longiflora var. tubiformis</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
   </si>
   <si>
     <t>Primula involucrata</t>
-  </si>
-  <si>
-    <t>Calamogrostis holciformis</t>
   </si>
   <si>
     <t>Festuca olgae</t>
@@ -464,6 +458,15 @@
   </si>
   <si>
     <t>Blysmus compressus</t>
+  </si>
+  <si>
+    <t>Calamagrostis holciformis</t>
+  </si>
+  <si>
+    <t>Lomatogonium brachyantherum</t>
+  </si>
+  <si>
+    <t>The category column is not used in the analysis</t>
   </si>
 </sst>
 </file>
@@ -614,10 +617,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -939,11 +938,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6620C268-8E80-43C7-B6DC-8822E5B4B5D3}">
   <dimension ref="A1:DD208"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BP8" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="CO35" sqref="A35:CO38"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,280 +956,280 @@
   <sheetData>
     <row r="1" spans="1:93" s="1" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="O1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BD1" s="13" t="s">
+      <c r="BF1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BK1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BM1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CK1" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="CK1" s="13" t="s">
+      <c r="CM1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="CM1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="CN1" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:93" x14ac:dyDescent="0.25">
@@ -1238,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1342,10 +1341,10 @@
     </row>
     <row r="3" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1452,7 +1451,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1569,7 +1568,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1718,7 +1717,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
@@ -1873,7 +1872,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1988,7 +1987,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -2102,10 +2101,10 @@
     </row>
     <row r="9" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>10</v>
+        <v>127</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -2207,10 +2206,10 @@
     </row>
     <row r="10" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -2320,10 +2319,10 @@
     </row>
     <row r="11" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -2421,10 +2420,10 @@
     </row>
     <row r="12" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -2522,10 +2521,10 @@
     </row>
     <row r="13" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2625,10 +2624,10 @@
     </row>
     <row r="14" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -2744,10 +2743,10 @@
     </row>
     <row r="15" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2853,10 +2852,10 @@
     </row>
     <row r="16" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3">
         <v>90</v>
@@ -3033,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -3160,7 +3159,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -3299,7 +3298,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3">
@@ -3440,7 +3439,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -3580,10 +3579,10 @@
     </row>
     <row r="21" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -3696,10 +3695,10 @@
     </row>
     <row r="22" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -3823,10 +3822,10 @@
     </row>
     <row r="23" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2">
         <v>5</v>
@@ -3982,10 +3981,10 @@
     </row>
     <row r="24" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>27</v>
+        <v>126</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -4097,10 +4096,10 @@
     </row>
     <row r="25" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -4200,10 +4199,10 @@
     </row>
     <row r="26" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -4303,10 +4302,10 @@
     </row>
     <row r="27" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -4404,10 +4403,10 @@
     </row>
     <row r="28" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -4509,10 +4508,10 @@
     </row>
     <row r="29" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -4628,10 +4627,10 @@
     </row>
     <row r="30" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -4739,10 +4738,10 @@
     </row>
     <row r="31" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="3">
@@ -5993,9 +5992,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CAEA5A-97D1-4AED-AE80-95CAA6A7C200}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -6003,12 +6002,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>